<commit_message>
ADO->FS ID field key
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{285D0283-FE72-4249-AA96-32321EC103CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70336A15-841B-4762-9C97-3D4EDFAAFB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
   <si>
     <t>FS-Field-Key</t>
   </si>
@@ -69,13 +69,13 @@
     <t>created_at</t>
   </si>
   <si>
-    <t>IMSCreatedOn</t>
+    <t>Custom.IMSCreatedOn</t>
   </si>
   <si>
     <t>queued_on</t>
   </si>
   <si>
-    <t>IMSQueuedOn</t>
+    <t>Custom.IMSQueuedOn</t>
   </si>
   <si>
     <t>product_version</t>
@@ -96,22 +96,19 @@
     <t>Custom.AccountID</t>
   </si>
   <si>
-    <t>source_control_reference</t>
+    <t>source_control_reference_created_on</t>
+  </si>
+  <si>
+    <t>System.CreatedDate</t>
   </si>
   <si>
     <t>ADO_TO_FS</t>
   </si>
   <si>
-    <t>source_control_reference_created_on</t>
-  </si>
-  <si>
-    <t>System.CreatedDate</t>
-  </si>
-  <si>
     <t>devops_status</t>
   </si>
   <si>
-    <t>System. State</t>
+    <t>System.State</t>
   </si>
   <si>
     <t>isMultiSelectFS</t>
@@ -796,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD10"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,38 +927,24 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -990,21 +973,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1016,7 +999,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -1024,7 +1007,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -1036,7 +1019,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1044,7 +1027,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1056,7 +1039,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1064,7 +1047,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1076,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1104,21 +1087,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1127,12 +1110,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -1141,12 +1124,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1155,12 +1138,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1169,12 +1152,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -1183,12 +1166,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>22</v>
@@ -1197,12 +1180,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1211,35 +1194,35 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1247,7 +1230,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1255,7 +1238,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1263,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1287,18 +1270,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1315,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1340,10 +1323,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -1351,10 +1334,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
@@ -1362,10 +1345,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
@@ -1373,10 +1356,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -1384,10 +1367,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -1395,10 +1378,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -1431,288 +1414,288 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="H9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AreaPath Iteration values edited in excel file
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94D5359C-DC03-4DA2-AB27-807041BD421D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF186B50-BBEC-47C7-9358-AC17499DBBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleField" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="83">
   <si>
     <t>FS-Field-Key</t>
   </si>
@@ -246,19 +246,13 @@
     <t>4.0.0.0</t>
   </si>
   <si>
-    <t>vg-test\VLMSV4</t>
-  </si>
-  <si>
-    <t>iteration1</t>
-  </si>
-  <si>
     <t>VG-SUPPORT-TEST</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>tester1</t>
+    <t>valgenesis\\Bharadwaj</t>
+  </si>
+  <si>
+    <t>valgenesis\\jayaraj</t>
   </si>
   <si>
     <t>Bug</t>
@@ -267,97 +261,31 @@
     <t>4.0.1</t>
   </si>
   <si>
-    <t>iternaltion2</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>tester2</t>
-  </si>
-  <si>
     <t>4.1.0.</t>
   </si>
   <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>tester3</t>
-  </si>
-  <si>
     <t>4.2.0</t>
   </si>
   <si>
-    <t>user4</t>
-  </si>
-  <si>
-    <t>tester4</t>
-  </si>
-  <si>
     <t>4.2.3</t>
   </si>
   <si>
-    <t>user5</t>
-  </si>
-  <si>
-    <t>tester5</t>
-  </si>
-  <si>
     <t>4.2.7</t>
   </si>
   <si>
-    <t>user6</t>
-  </si>
-  <si>
-    <t>tester6</t>
-  </si>
-  <si>
     <t>5.0.0.0.</t>
   </si>
   <si>
-    <t>vg-test\VLMSV5</t>
-  </si>
-  <si>
-    <t>user7</t>
-  </si>
-  <si>
-    <t>tester7</t>
-  </si>
-  <si>
     <t>5.1.0.0.</t>
   </si>
   <si>
-    <t>user8</t>
-  </si>
-  <si>
-    <t>tester8</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
     <t>1.5.0.3.</t>
   </si>
   <si>
-    <t>vg-test\PM</t>
-  </si>
-  <si>
-    <t>user9</t>
-  </si>
-  <si>
-    <t>tester9</t>
-  </si>
-  <si>
     <t>4.1.1.17</t>
-  </si>
-  <si>
-    <t>iteration4</t>
-  </si>
-  <si>
-    <t>user10</t>
-  </si>
-  <si>
-    <t>tester10</t>
   </si>
 </sst>
 </file>
@@ -795,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1396,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930C70B-AF26-4906-A7FA-5CFF610F4C06}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1405,10 +1333,10 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1445,23 +1373,23 @@
       <c r="B2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75">
@@ -1469,25 +1397,25 @@
         <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
@@ -1495,25 +1423,25 @@
         <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75">
@@ -1521,25 +1449,25 @@
         <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75">
@@ -1547,25 +1475,25 @@
         <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75">
@@ -1573,25 +1501,25 @@
         <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75">
@@ -1599,25 +1527,25 @@
         <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75">
@@ -1625,51 +1553,51 @@
         <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="H9" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75">
@@ -1677,25 +1605,25 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>100</v>
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extra slash removed in developer tester name in excel file
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF186B50-BBEC-47C7-9358-AC17499DBBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{384357F9-C160-44D5-8253-54E598461D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,10 +249,10 @@
     <t>VG-SUPPORT-TEST</t>
   </si>
   <si>
-    <t>valgenesis\\Bharadwaj</t>
-  </si>
-  <si>
-    <t>valgenesis\\jayaraj</t>
+    <t>valgenesis\Bharadwaj</t>
+  </si>
+  <si>
+    <t>valgenesis\jayaraj</t>
   </si>
   <si>
     <t>Bug</t>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G2" sqref="G2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added AssignedTo and fixed circular bug dependency in logger
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{384357F9-C160-44D5-8253-54E598461D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8538964A-A5B1-4EF3-ABAF-58D57FC4BC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="85">
   <si>
     <t>FS-Field-Key</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>WorkItemType</t>
+  </si>
+  <si>
+    <t>System.AssignedTo</t>
+  </si>
+  <si>
+    <t>AssignedTo</t>
   </si>
   <si>
     <t>ProductName</t>
@@ -1222,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB14AF16-485B-4CEC-8C39-B447C30A7282}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1315,6 +1321,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1322,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930C70B-AF26-4906-A7FA-5CFF610F4C06}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G11"/>
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1337,15 +1354,16 @@
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>59</v>
@@ -1363,267 +1381,300 @@
         <v>57</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75">
+      <c r="H3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75">
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75">
+        <v>73</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date type for fs fields. removed logger debug.
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8538964A-A5B1-4EF3-ABAF-58D57FC4BC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20B5F932-3CEF-40A4-9814-86025E231D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleField" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="86">
   <si>
     <t>FS-Field-Key</t>
   </si>
@@ -51,6 +51,9 @@
     <t>Direction</t>
   </si>
   <si>
+    <t>FS-Field-Type</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -66,12 +69,18 @@
     <t>System.Title</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
     <t>created_at</t>
   </si>
   <si>
     <t>Custom.IMSCreatedOn</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>queued_on</t>
   </si>
   <si>
@@ -103,12 +112,6 @@
   </si>
   <si>
     <t>ADO_TO_FS</t>
-  </si>
-  <si>
-    <t>devops_status</t>
-  </si>
-  <si>
-    <t>System.State</t>
   </si>
   <si>
     <t>isMultiSelectFS</t>
@@ -727,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,9 +742,10 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,131 +758,138 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -907,21 +918,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -930,10 +941,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -941,7 +952,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -950,10 +961,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -961,7 +972,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -970,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -981,7 +992,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -990,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1021,21 +1032,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1044,12 +1055,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -1058,12 +1069,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -1072,12 +1083,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1086,12 +1097,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -1100,12 +1111,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>22</v>
@@ -1114,12 +1125,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1128,59 +1139,59 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1204,18 +1215,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1257,79 +1268,79 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1341,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930C70B-AF26-4906-A7FA-5CFF610F4C06}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1360,321 +1371,321 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="I1" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prodVersion, name find. remove query sheet
</commit_message>
<xml_diff>
--- a/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
+++ b/apps/scheduler/data/VG-FS-ADO-Sync.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20B5F932-3CEF-40A4-9814-86025E231D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07EA1094-2390-48FA-9428-2598ABC219D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleField" sheetId="1" r:id="rId1"/>
     <sheet name="Repo" sheetId="2" r:id="rId2"/>
-    <sheet name="Query" sheetId="3" r:id="rId3"/>
-    <sheet name="URL" sheetId="7" r:id="rId4"/>
-    <sheet name="ProductsFields" sheetId="4" r:id="rId5"/>
-    <sheet name="ProductsData" sheetId="6" r:id="rId6"/>
-    <sheet name="Attachments" sheetId="5" r:id="rId7"/>
+    <sheet name="URL" sheetId="7" r:id="rId3"/>
+    <sheet name="ProductsFields" sheetId="4" r:id="rId4"/>
+    <sheet name="ProductsData" sheetId="6" r:id="rId5"/>
+    <sheet name="Attachments" sheetId="5" r:id="rId6"/>
+    <sheet name="TextFields" sheetId="8" r:id="rId7"/>
+    <sheet name="TextFieldsData" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="86">
   <si>
     <t>FS-Field-Key</t>
   </si>
@@ -99,7 +100,7 @@
     <t>Custom.Solution</t>
   </si>
   <si>
-    <t>department_id</t>
+    <t>department_name</t>
   </si>
   <si>
     <t>Custom.AccountID</t>
@@ -114,6 +115,12 @@
     <t>ADO_TO_FS</t>
   </si>
   <si>
+    <t>devops_status</t>
+  </si>
+  <si>
+    <t>System.State</t>
+  </si>
+  <si>
     <t>isMultiSelectFS</t>
   </si>
   <si>
@@ -147,111 +154,72 @@
     <t>Problem Statement</t>
   </si>
   <si>
-    <t>Param</t>
+    <t>Key</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>isValueBoolean</t>
-  </si>
-  <si>
-    <t>EnclosingQuotesType</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>SINGLE_QUOTES</t>
-  </si>
-  <si>
-    <t>workspace_id</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>queued_with</t>
-  </si>
-  <si>
-    <t>Level-3</t>
-  </si>
-  <si>
-    <t>Disable_DevOps_Sync</t>
-  </si>
-  <si>
-    <t>f</t>
+    <t>FS_FETCH_QUERY</t>
+  </si>
+  <si>
+    <t>(status:'12' OR status:'14' OR  status:'17' OR status:'20' OR status:'21' OR status:'22') AND workspace_id:3 AND queued_with: 'Level-3' AND Disable_DevOps_Sync:false</t>
+  </si>
+  <si>
+    <t>ProductsDataSheetKey</t>
+  </si>
+  <si>
+    <t>Custom.Developer</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Custom.Tester</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>System.AreaPath</t>
+  </si>
+  <si>
+    <t>AreaPath</t>
+  </si>
+  <si>
+    <t>System.TeamProject</t>
+  </si>
+  <si>
+    <t>TeamProject</t>
+  </si>
+  <si>
+    <t>System.IterationPath</t>
+  </si>
+  <si>
+    <t>IterationPath</t>
+  </si>
+  <si>
+    <t>System.WorkItemType</t>
+  </si>
+  <si>
+    <t>WorkItemType</t>
+  </si>
+  <si>
+    <t>System.AssignedTo</t>
+  </si>
+  <si>
+    <t>AssignedTo</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductVersion</t>
   </si>
   <si>
     <t>VLMS</t>
   </si>
   <si>
-    <t>PLS</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>FS_FETCH_QUERY</t>
-  </si>
-  <si>
-    <t>(status:'12' OR status:'14' OR  status:'17' OR status:'20' OR status:'21' OR status:'22') AND workspace_id:3 AND queued_with: 'Level-3' AND Disable_DevOps_Sync:false</t>
-  </si>
-  <si>
-    <t>ProductsDataSheetKey</t>
-  </si>
-  <si>
-    <t>Custom.Developer</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>Custom.Tester</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>System.AreaPath</t>
-  </si>
-  <si>
-    <t>AreaPath</t>
-  </si>
-  <si>
-    <t>System.TeamProject</t>
-  </si>
-  <si>
-    <t>TeamProject</t>
-  </si>
-  <si>
-    <t>System.IterationPath</t>
-  </si>
-  <si>
-    <t>IterationPath</t>
-  </si>
-  <si>
-    <t>System.WorkItemType</t>
-  </si>
-  <si>
-    <t>WorkItemType</t>
-  </si>
-  <si>
-    <t>System.AssignedTo</t>
-  </si>
-  <si>
-    <t>AssignedTo</t>
-  </si>
-  <si>
-    <t>ProductName</t>
-  </si>
-  <si>
-    <t>ProductVersion</t>
-  </si>
-  <si>
     <t>4.0.0.0</t>
   </si>
   <si>
@@ -295,6 +263,39 @@
   </si>
   <si>
     <t>4.1.1.17</t>
+  </si>
+  <si>
+    <t>CustomDataSheetKey</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Custom.IMSPriority</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>FieldObject</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>If no name, just put ID</t>
   </si>
 </sst>
 </file>
@@ -348,12 +349,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -384,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -395,6 +402,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -730,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,6 +898,23 @@
       </c>
       <c r="E9" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -918,21 +943,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -944,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -952,7 +977,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
@@ -964,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -972,7 +997,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -984,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -992,7 +1017,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1004,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1016,190 +1041,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25196F1-1288-4BD5-BDF0-33BE169FEFB5}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>17</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>21</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230A98D7-5B57-4F8B-BC33-6C44C99262A8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1215,18 +1056,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB14AF16-485B-4CEC-8C39-B447C30A7282}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1260,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1268,10 +1109,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1279,10 +1120,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1290,10 +1131,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -1301,10 +1142,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -1312,10 +1153,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -1323,10 +1164,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
@@ -1334,13 +1175,361 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930C70B-AF26-4906-A7FA-5CFF610F4C06}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75">
+      <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75">
+      <c r="A3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
+      <c r="A4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
+      <c r="A6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
+      <c r="A8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
+      <c r="A9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
+      <c r="A10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1349,351 +1538,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930C70B-AF26-4906-A7FA-5CFF610F4C06}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4D7874-454C-4EAC-98C9-E36175A7C2FD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1703,4 +1547,142 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC8DB2D-8624-4D05-9780-94E3A2BB9405}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7161C4D0-8C10-42FC-9BEE-EF847D626502}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="10">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>